<commit_message>
change int to float
</commit_message>
<xml_diff>
--- a/strategy.xlsx
+++ b/strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gamescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6636E5D5-4EE3-45E8-AA25-379F04D0F506}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D70ACF8-8FC3-4A5F-B098-7EF9C6D008BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7890" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>第一面</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,6 +124,10 @@
   </si>
   <si>
     <t>（不使用技能可以不填也可以填0）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（若技能需要使用，该列一定要进行填写）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -494,7 +498,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -511,7 +515,9 @@
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -677,7 +683,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -694,7 +700,9 @@
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -847,7 +855,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -864,7 +872,9 @@
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
add the function to check the fight side
</commit_message>
<xml_diff>
--- a/strategy.xlsx
+++ b/strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gamescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D70ACF8-8FC3-4A5F-B098-7EF9C6D008BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E7F202-25C6-4E8D-AAD1-01F5D51CA2BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7890" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change keyboard press to mouse press
</commit_message>
<xml_diff>
--- a/strategy.xlsx
+++ b/strategy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gamescript\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gamescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8852CBA7-BA5A-4109-8B75-63D8562589AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC0749-F00B-406F-AE99-1699B9EE5A7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7890" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="7896" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>第一面</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,7 +168,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>QP</t>
+    <t>bondage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟器窗口名称（默认为网易mumu模拟器）：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命运-冠位指定 - MuMu模拟器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,40 +554,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4132F87-1379-47FC-B3E4-A9BB87BCDE53}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="123.125" customWidth="1"/>
+    <col min="1" max="1" width="123.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -587,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -595,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -603,15 +612,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -619,12 +628,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -639,17 +656,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
-    <col min="3" max="3" width="68.25" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -671,7 +688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -682,92 +699,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -778,7 +787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -789,21 +798,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -812,7 +821,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
@@ -828,17 +837,17 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -849,7 +858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -860,91 +869,111 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -955,7 +984,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -966,21 +995,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1000,17 +1029,17 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.75" customWidth="1"/>
-    <col min="2" max="2" width="28.75" customWidth="1"/>
-    <col min="3" max="3" width="72.875" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+    <col min="3" max="3" width="72.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1021,7 +1050,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1032,91 +1061,99 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1127,32 +1164,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1163,5 +1200,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add function to change character
</commit_message>
<xml_diff>
--- a/strategy.xlsx
+++ b/strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gamescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC0749-F00B-406F-AE99-1699B9EE5A7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B00FCD-C5D5-4A73-80FE-ABB7F8E20E29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="7896" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7890" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
   <si>
     <t>第一面</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,9 +67,6 @@
     <t>御主装备技能2</t>
   </si>
   <si>
-    <t>御主装备技能3</t>
-  </si>
-  <si>
     <t>技能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -177,6 +174,30 @@
   </si>
   <si>
     <t>命运-冠位指定 - MuMu模拟器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kongming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>换上角色技能1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>御主衣服为换人礼装（1为是，0为否）：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>换上角色技能2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>换上角色技能3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>御主装备技能3（若为换人，C列输入换下角色编号（1,2,3），D列输入换上角色编号（4,5,6））</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -554,94 +575,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4132F87-1379-47FC-B3E4-A9BB87BCDE53}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="123.109375" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
+    <col min="1" max="1" width="123.125" customWidth="1"/>
+    <col min="2" max="2" width="29.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="B7" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
-        <v>38</v>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -653,42 +682,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3CA7D3-8162-4A38-A0A5-38F2F52A01A4}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="68.21875" customWidth="1"/>
+    <col min="1" max="1" width="82.125" customWidth="1"/>
+    <col min="2" max="2" width="29.875" customWidth="1"/>
+    <col min="3" max="3" width="68.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -699,131 +728,152 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1">
         <v>27</v>
       </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -834,56 +884,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48348C4C-F706-4CF7-8E15-549AF4687FC5}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A14" sqref="A14:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="81.375" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -894,21 +944,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -919,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -930,21 +980,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
@@ -952,68 +1002,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1">
         <v>27</v>
       </c>
     </row>
@@ -1026,63 +1097,63 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94A6540-5647-411E-BD19-D1EF0227C28B}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="72.88671875" customWidth="1"/>
+    <col min="1" max="1" width="81.5" customWidth="1"/>
+    <col min="2" max="2" width="28.75" customWidth="1"/>
+    <col min="3" max="3" width="72.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1093,49 +1164,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1146,54 +1217,94 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix one bug in checking character
</commit_message>
<xml_diff>
--- a/strategy.xlsx
+++ b/strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gamescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B00FCD-C5D5-4A73-80FE-ABB7F8E20E29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404B8EFD-1D18-458D-9E38-E7EDDE2DDB0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7890" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
   </bookViews>
@@ -578,7 +578,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -670,7 +670,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1097,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94A6540-5647-411E-BD19-D1EF0227C28B}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1110,7 @@
     <col min="3" max="3" width="72.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1132,28 +1132,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1164,49 +1164,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1217,52 +1217,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">

</xml_diff>

<commit_message>
fix bug of the interval in changing character
</commit_message>
<xml_diff>
--- a/strategy.xlsx
+++ b/strategy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gamescript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fgo\gamescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404B8EFD-1D18-458D-9E38-E7EDDE2DDB0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE4205F-EF3F-4F34-A00B-3637F938958F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7890" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="7896" activeTab="1" xr2:uid="{D09C6AC7-655D-4B1E-A499-4EBA821291C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
   <si>
     <t>第一面</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -165,22 +165,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bondage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>模拟器窗口名称（默认为网易mumu模拟器）：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>命运-冠位指定 - MuMu模拟器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kongming</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>换上角色技能1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,6 +186,14 @@
   </si>
   <si>
     <t>御主装备技能3（若为换人，C列输入换下角色编号（1,2,3），D列输入换上角色编号（4,5,6））</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷电模拟器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -577,71 +573,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4132F87-1379-47FC-B3E4-A9BB87BCDE53}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="123.125" customWidth="1"/>
-    <col min="2" max="2" width="29.125" customWidth="1"/>
+    <col min="1" max="1" width="123.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -649,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -657,20 +653,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -682,20 +678,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3CA7D3-8162-4A38-A0A5-38F2F52A01A4}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.125" customWidth="1"/>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
-    <col min="3" max="3" width="68.25" customWidth="1"/>
+    <col min="1" max="1" width="82.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="68.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -717,7 +713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -728,105 +724,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -837,7 +864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -848,30 +875,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
     </row>
@@ -886,18 +913,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48348C4C-F706-4CF7-8E15-549AF4687FC5}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="81.375" customWidth="1"/>
+    <col min="1" max="1" width="81.33203125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -908,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -919,132 +946,112 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -1055,7 +1062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1066,26 +1073,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1099,18 +1106,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94A6540-5647-411E-BD19-D1EF0227C28B}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="81.5" customWidth="1"/>
-    <col min="2" max="2" width="28.75" customWidth="1"/>
-    <col min="3" max="3" width="72.875" customWidth="1"/>
+    <col min="1" max="1" width="81.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+    <col min="3" max="3" width="72.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1121,7 +1128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1132,120 +1139,120 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -1256,32 +1263,32 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>